<commit_message>
Update qualitative assessment to latest version
This version has been used to generate final figures in the manuscript
</commit_message>
<xml_diff>
--- a/qualitative_assessment/qualitative_assessment.xlsx
+++ b/qualitative_assessment/qualitative_assessment.xlsx
@@ -118,7 +118,7 @@
     <t xml:space="preserve">sub-9604_run-1_T2starw.nii.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">CHUM (9604)</t>
+    <t xml:space="preserve">Philips (9604)</t>
   </si>
   <si>
     <t xml:space="preserve">sub-9604_run-2_T2starw.nii.gz</t>
@@ -139,40 +139,40 @@
     <t xml:space="preserve">sub-9605_run-2_T2starw.nii.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">sub-9611</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9611_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxford (9611)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9611_run-2_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9612</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9612_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxford (9612)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9612_run-2_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9613</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9613_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxford (9613)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9613_run-2_T2starw.nii.gz</t>
+    <t xml:space="preserve">sub-9611Ses1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses1_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxford (9611Ses1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses1_run-2_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses2_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxford (9611Ses2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses2_run-2_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses3_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxford (9611Ses3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses3_run-2_T2starw.nii.gz</t>
   </si>
   <si>
     <t xml:space="preserve">sub-9669</t>
@@ -187,55 +187,55 @@
     <t xml:space="preserve">sub-9669_run-2_T2starw.nii.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">sub-9709</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9709_run-1_T2starw.nii.gz</t>
+    <t xml:space="preserve">sub-9709Ses1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9709Ses1_run-1_T2starw.nii.gz</t>
   </si>
   <si>
     <t xml:space="preserve">1.5T</t>
   </si>
   <si>
-    <t xml:space="preserve">Milan (9709)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9709_run-2_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9710</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9710_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milan (9710)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9710_run-2_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10062_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEITEC (10062)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10062_run-2_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10063_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEITEC (10063)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10063_run-2_T2starw.nii.gz</t>
+    <t xml:space="preserve">Milan (9709Ses1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9709Ses1_run-2_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9709Ses2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9709Ses2_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milan (9709Ses2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9709Ses2_run-2_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses1_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEITEC (10062Ses1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses1_run-2_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses2_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEITEC (10062Ses2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses2_run-2_T2starw.nii.gz</t>
   </si>
   <si>
     <t xml:space="preserve">sub-20210728</t>
@@ -375,17 +375,17 @@
   </sheetPr>
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O33" activeCellId="0" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.93"/>
@@ -393,10 +393,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="43.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="43.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="18.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="1" width="55.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="18.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="55.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update qualitative assessment code (#67)
* Create qualitative_assessment.m

MATLAB function generating graph of qualitative assessment shown in gm-challenge paper.
Example call as: qualitative_assessment('qualitative_assessment.xlsx')
Or example call from terminal generating figure_qualitative_assessment.png file:
matlab -r "qualitative_assessment('qualitative_assessment.xlsx'),print('figure_qualitative_assessment', '-dpng', '-r300'),pause(0.5),exit"

* Add sheet qualitative_assessment.xlsx

Source sheet for the function qualitative_assessment.m

* Update qualitative assessment to latest version

This version has been used to generate final figures in the manuscript
</commit_message>
<xml_diff>
--- a/qualitative_assessment/qualitative_assessment.xlsx
+++ b/qualitative_assessment/qualitative_assessment.xlsx
@@ -118,7 +118,7 @@
     <t xml:space="preserve">sub-9604_run-1_T2starw.nii.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">CHUM (9604)</t>
+    <t xml:space="preserve">Philips (9604)</t>
   </si>
   <si>
     <t xml:space="preserve">sub-9604_run-2_T2starw.nii.gz</t>
@@ -139,40 +139,40 @@
     <t xml:space="preserve">sub-9605_run-2_T2starw.nii.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">sub-9611</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9611_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxford (9611)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9611_run-2_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9612</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9612_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxford (9612)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9612_run-2_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9613</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9613_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxford (9613)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9613_run-2_T2starw.nii.gz</t>
+    <t xml:space="preserve">sub-9611Ses1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses1_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxford (9611Ses1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses1_run-2_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses2_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxford (9611Ses2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses2_run-2_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses3_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxford (9611Ses3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9611Ses3_run-2_T2starw.nii.gz</t>
   </si>
   <si>
     <t xml:space="preserve">sub-9669</t>
@@ -187,55 +187,55 @@
     <t xml:space="preserve">sub-9669_run-2_T2starw.nii.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">sub-9709</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9709_run-1_T2starw.nii.gz</t>
+    <t xml:space="preserve">sub-9709Ses1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9709Ses1_run-1_T2starw.nii.gz</t>
   </si>
   <si>
     <t xml:space="preserve">1.5T</t>
   </si>
   <si>
-    <t xml:space="preserve">Milan (9709)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9709_run-2_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9710</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9710_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milan (9710)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-9710_run-2_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10062_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEITEC (10062)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10062_run-2_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10063_run-1_T2starw.nii.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEITEC (10063)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub-10063_run-2_T2starw.nii.gz</t>
+    <t xml:space="preserve">Milan (9709Ses1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9709Ses1_run-2_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9709Ses2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9709Ses2_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milan (9709Ses2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-9709Ses2_run-2_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses1_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEITEC (10062Ses1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses1_run-2_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses2_run-1_T2starw.nii.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEITEC (10062Ses2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-10062Ses2_run-2_T2starw.nii.gz</t>
   </si>
   <si>
     <t xml:space="preserve">sub-20210728</t>
@@ -375,17 +375,17 @@
   </sheetPr>
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O33" activeCellId="0" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.93"/>
@@ -393,10 +393,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="43.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="43.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="18.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="1" width="55.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="18.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="55.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>